<commit_message>
all api - error-message/ permission
</commit_message>
<xml_diff>
--- a/seeders/seed_data.xlsx
+++ b/seeders/seed_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e62788ad37f281/바탕 화면/projects/work/node_server/seeders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_2E8F6F78A56906AE739E887464DCC40DD82B21BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D264B378-6EFD-427F-A174-9AC1A8A1B2ED}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="11_2E8F6F78A56906AE739E887464DCC40DD82B21BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E97F0B67-6B66-4177-B2B6-35153B295181}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21624" windowHeight="11244" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="2" r:id="rId1"/>
     <sheet name="ErrorMessages" sheetId="4" r:id="rId2"/>
     <sheet name="Permissions" sheetId="3" r:id="rId3"/>
+    <sheet name="API" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>migration</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -182,6 +183,56 @@
   </si>
   <si>
     <t>moduler/user_update.patch_info</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>apiId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST/user</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET/user</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PATCH/user</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE/user</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET/user/ids</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>all_api/permission</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>권한없음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unauthorized</t>
+  </si>
+  <si>
+    <t>api not found (no match entry-point)</t>
+  </si>
+  <si>
+    <t>존재하지 않는 api</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1+B2:B21</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -189,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -214,6 +265,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF6D6D6D"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -235,12 +293,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -577,10 +636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB3323-D0E3-45B1-AD6D-E98237329D30}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -614,8 +673,8 @@
       <c r="A2" t="b">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -876,7 +935,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -890,7 +949,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -904,7 +963,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -918,11 +977,48 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C21" s="1"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>401.1</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>404</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -933,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85279200-1977-43D4-AD14-060D07B2F8C2}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -965,6 +1061,99 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4D7948-5FAD-4C0C-B1FB-544C8C77BB1B}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="15.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change state to simple Column
</commit_message>
<xml_diff>
--- a/seeders/seed_data.xlsx
+++ b/seeders/seed_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e62788ad37f281/바탕 화면/projects/work/node_server/seeders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D41B787-94AD-4676-8831-A4BEB72FC323}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13400279-0CE5-471D-B684-1C6E31650674}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Status" sheetId="2" r:id="rId1"/>
+    <sheet name="Status" sheetId="6" r:id="rId1"/>
     <sheet name="ErrorMessages" sheetId="4" r:id="rId2"/>
     <sheet name="Permissions" sheetId="3" r:id="rId3"/>
     <sheet name="API" sheetId="5" r:id="rId4"/>
+    <sheet name="Status_1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>migration</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -278,6 +279,10 @@
   </si>
   <si>
     <t>GET/permission/api/DB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -620,62 +625,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A70233-D52E-4397-96AB-A873070A9064}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CF54BD-6A96-4857-852A-D5B80E62C6E3}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="b">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="b">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="b">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1129,9 +1123,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85279200-1977-43D4-AD14-060D07B2F8C2}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -1167,6 +1161,11 @@
       </c>
       <c r="B4" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.4">
+      <c r="F24" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4D7948-5FAD-4C0C-B1FB-544C8C77BB1B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1368,4 +1367,64 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A70233-D52E-4397-96AB-A873070A9064}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactor m:n field name
</commit_message>
<xml_diff>
--- a/seeders/seed_data.xlsx
+++ b/seeders/seed_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e62788ad37f281/바탕 화면/projects/work/node_server/seeders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39A2F42A-34E3-4AD0-B7C0-DAA62066BB68}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F77F24A-E426-4331-9EC5-11CD5905EA51}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -123,19 +123,12 @@
     <t>bulkCreate</t>
   </si>
   <si>
-    <t>modules/user_password.logUp</t>
-  </si>
-  <si>
     <t>생성실패</t>
   </si>
   <si>
     <t>UserPermissionCreate Error</t>
   </si>
   <si>
-    <t>modules/user_password.logIn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>wrongInput</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -160,30 +153,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>modules/user_search.all</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>modules/user_search.choice</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>modules/user_search.search_init</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>modules/user_search.search_include</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>moduler/user_update.patch_user</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>moduler/user_update.patch_info</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>apiId</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -291,6 +260,38 @@
   </si>
   <si>
     <t>different creater</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.password.logUp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.password.logIn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>moduler/user.update.patch_user</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>moduler/user.update.patch_info</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.search.search_include</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.search.search_init</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.search.choice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.search.all</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -685,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB3323-D0E3-45B1-AD6D-E98237329D30}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -802,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>400</v>
@@ -819,7 +820,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>400</v>
@@ -835,14 +836,14 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8">
+        <v>400</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8">
-        <v>400</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -852,14 +853,14 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
@@ -870,16 +871,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <v>400</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -890,13 +891,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D11">
-        <v>400</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -908,16 +909,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>400</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
@@ -928,16 +929,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D13">
         <v>400</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
@@ -948,7 +949,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="D14">
         <v>400</v>
@@ -962,7 +963,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>400</v>
@@ -977,7 +978,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>400</v>
@@ -991,7 +992,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="D17">
         <v>400</v>
@@ -1005,7 +1006,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D18">
         <v>400</v>
@@ -1019,7 +1020,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>400</v>
@@ -1033,16 +1034,16 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>401.1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -1053,16 +1054,16 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>404</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
@@ -1073,16 +1074,16 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D22">
         <v>400</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
@@ -1093,7 +1094,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D23">
         <v>400</v>
@@ -1110,7 +1111,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D24">
         <v>400</v>
@@ -1127,16 +1128,16 @@
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D25">
         <v>400</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
@@ -1147,13 +1148,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D26">
         <v>400</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
@@ -1164,13 +1165,13 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D27">
         <v>400</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.4">
@@ -1235,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4D7948-5FAD-4C0C-B1FB-544C8C77BB1B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1246,7 +1247,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1257,10 +1258,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1268,10 +1269,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1279,7 +1280,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1290,7 +1291,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1301,7 +1302,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -1312,7 +1313,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -1323,10 +1324,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1334,10 +1335,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1345,10 +1346,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -1356,10 +1357,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -1367,10 +1368,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -1378,7 +1379,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -1389,7 +1390,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -1400,7 +1401,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -1411,7 +1412,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
refactor user_update -> Class User
</commit_message>
<xml_diff>
--- a/seeders/seed_data.xlsx
+++ b/seeders/seed_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e62788ad37f281/바탕 화면/projects/work/node_server/seeders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F77F24A-E426-4331-9EC5-11CD5905EA51}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C814012-0E77-4179-A4D4-05AD925A8A1B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5424" yWindow="2448" windowWidth="17280" windowHeight="8880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>migration</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -251,10 +251,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>modeuls/article.patchArticle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Not Found Article Id</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -292,6 +288,38 @@
   </si>
   <si>
     <t>modules/user.search.all</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB쪽 오류가능성 높음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>defaultValue</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/article.patchArticle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.user.disactive</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modulse/user.User.patch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>email,password 미변동</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modulse/user.UserInfo.patch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>birthday,intro 미변동</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -638,7 +666,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -684,494 +712,468 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB3323-D0E3-45B1-AD6D-E98237329D30}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="48.59765625" customWidth="1"/>
-    <col min="4" max="4" width="13.8984375" customWidth="1"/>
-    <col min="5" max="5" width="25.59765625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="48.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.8984375" customWidth="1"/>
+    <col min="4" max="4" width="25.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>400</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>419</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>401</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>400</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11">
+        <v>400</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12">
+        <v>400</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13">
+        <v>400</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" t="b">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="D2">
-        <v>400</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3">
-        <v>419</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>401</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>401.1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" t="b">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>400</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" t="b">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6">
-        <v>400</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22">
+        <v>404</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" t="b">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7">
-        <v>400</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23">
+        <v>400</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" t="b">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8">
-        <v>400</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24">
+        <v>400</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25">
+        <v>400</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10" t="b">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10">
-        <v>400</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26">
+        <v>400</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" t="b">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11">
-        <v>400</v>
-      </c>
-      <c r="E11" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>400</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" t="b">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12">
-        <v>400</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28">
+        <v>400</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29">
+        <v>400</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A13" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13">
-        <v>400</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <v>400</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A14" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A15" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15">
-        <v>400</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A16" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A17" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A18" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20">
-        <v>401.1</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A21" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21">
-        <v>404</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22" t="b">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22">
-        <v>400</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A23" t="b">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23">
-        <v>400</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" t="b">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24">
-        <v>400</v>
-      </c>
-      <c r="F24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25">
-        <v>400</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A26" t="b">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26">
-        <v>400</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27" t="b">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>26</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27">
-        <v>400</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>58</v>
+      <c r="B31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31">
+        <v>400</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add -log up with permission
</commit_message>
<xml_diff>
--- a/seeders/seed_data.xlsx
+++ b/seeders/seed_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e62788ad37f281/바탕 화면/projects/work/node_server/seeders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C814012-0E77-4179-A4D4-05AD925A8A1B}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D62A624-5728-45CA-B98F-5B25207DC535}"/>
   <bookViews>
     <workbookView xWindow="5424" yWindow="2448" windowWidth="17280" windowHeight="8880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
   <si>
     <t>migration</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -320,6 +320,14 @@
   </si>
   <si>
     <t>birthday,intro 미변동</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.User.LogUp- create user</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modules/user.User.LogUp- create user_permission</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -402,10 +410,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -714,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB3323-D0E3-45B1-AD6D-E98237329D30}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -868,10 +872,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -882,7 +886,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C11">
         <v>400</v>

</xml_diff>

<commit_message>
add kakao logup - login
</commit_message>
<xml_diff>
--- a/seeders/seed_data.xlsx
+++ b/seeders/seed_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e62788ad37f281/바탕 화면/projects/work/node_server/seeders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D62A624-5728-45CA-B98F-5B25207DC535}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="14_{5957F28C-072E-408C-B7BF-6C8D4581D32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBB66E0A-A686-41C2-9A60-ACCA83116689}"/>
   <bookViews>
     <workbookView xWindow="5424" yWindow="2448" windowWidth="17280" windowHeight="8880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
   <si>
     <t>migration</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -328,6 +328,14 @@
   </si>
   <si>
     <t>modules/user.User.LogUp- create user_permission</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>modulse/user.User.logIn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>deleted</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -410,6 +418,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -670,7 +682,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -716,10 +728,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB3323-D0E3-45B1-AD6D-E98237329D30}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1178,6 +1190,20 @@
       </c>
       <c r="D31" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32">
+        <v>400</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoer - ip check
</commit_message>
<xml_diff>
--- a/seeders/seed_data.xlsx
+++ b/seeders/seed_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakep\OneDrive\바탕 화면\projects\work\node_server\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B87887-ED3C-4E59-9F68-5EF28CC097D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1768FA8C-745F-4112-8336-707FA24B39E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -738,7 +738,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>